<commit_message>
This is the version 2 of converting now strings are converted to double
</commit_message>
<xml_diff>
--- a/Converting.xlsx
+++ b/Converting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4acb67461a0c26d7/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varun\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{AA58C895-B0AE-445A-B515-CFECBF655C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{107D1A44-CC34-46C0-A1D8-D605C0B6F06A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7F78BE-427A-4D3E-96BE-5E11E02A46B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -524,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{EA807800-7D99-42C2-8FA7-105696568FFD}">
+    <comment ref="A63" authorId="0" shapeId="0" xr:uid="{EA807800-7D99-42C2-8FA7-105696568FFD}">
       <text>
         <r>
           <rPr>
@@ -568,7 +568,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0" xr:uid="{6523EF89-7C7C-41DC-B9D8-92708814E2E3}">
+    <comment ref="B63" authorId="0" shapeId="0" xr:uid="{6523EF89-7C7C-41DC-B9D8-92708814E2E3}">
       <text>
         <r>
           <rPr>
@@ -633,7 +633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0" xr:uid="{4630BF63-60C7-42F9-9C60-EF9CD44B688A}">
+    <comment ref="C63" authorId="0" shapeId="0" xr:uid="{4630BF63-60C7-42F9-9C60-EF9CD44B688A}">
       <text>
         <r>
           <rPr>
@@ -659,7 +659,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D22" authorId="0" shapeId="0" xr:uid="{A8EDB628-DA3F-4BA1-A578-480C70A6FC27}">
+    <comment ref="D63" authorId="0" shapeId="0" xr:uid="{A8EDB628-DA3F-4BA1-A578-480C70A6FC27}">
       <text>
         <r>
           <rPr>
@@ -704,7 +704,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E22" authorId="0" shapeId="0" xr:uid="{A6607402-9B3D-4194-8CA9-39747FF47C55}">
+    <comment ref="E63" authorId="0" shapeId="0" xr:uid="{A6607402-9B3D-4194-8CA9-39747FF47C55}">
       <text>
         <r>
           <rPr>
@@ -728,7 +728,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+    <comment ref="F63" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
       <text>
         <r>
           <rPr>
@@ -751,7 +751,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+    <comment ref="G63" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
       <text>
         <r>
           <rPr>
@@ -793,7 +793,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="50">
   <si>
     <t>Program
 or module:</t>
@@ -920,12 +920,64 @@
   <si>
     <t>Version 3</t>
   </si>
+  <si>
+    <t>Varun Chhabra
+Date-8 Aug 2022</t>
+  </si>
+  <si>
+    <t>it's converting string to double integer so for alphabets it is showing 0</t>
+  </si>
+  <si>
+    <t>123abx.5678</t>
+  </si>
+  <si>
+    <t>to check the function for larger numbers</t>
+  </si>
+  <si>
+    <t>to check the function for larger numbers with decimals</t>
+  </si>
+  <si>
+    <t>it's converting the point one variables too because it is in double</t>
+  </si>
+  <si>
+    <t>to check the function for 15 digit number with 6 decimals</t>
+  </si>
+  <si>
+    <t>it's rounding off the decimal or some time it shows 0 only after the decimal this is because it is double</t>
+  </si>
+  <si>
+    <t xml:space="preserve">as it is double so it can only take 15 digit before points after that it stores the garbage characters  </t>
+  </si>
+  <si>
+    <t>to check the function with alpha- double numeric</t>
+  </si>
+  <si>
+    <t>to check the function with alpha-double numeric</t>
+  </si>
+  <si>
+    <t>To convert ten digit numeric string to double integer</t>
+  </si>
+  <si>
+    <t>To convert nine digit numeric string todouble  integer</t>
+  </si>
+  <si>
+    <t>To convert three digit numeric string to double integer</t>
+  </si>
+  <si>
+    <t>To convert one digit numeric string todouble  integer</t>
+  </si>
+  <si>
+    <t>as it is double so it can only take 15 digit before points and 6 digit after point it's rounding off that’s due to the precision error.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1227,7 +1279,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1314,6 +1366,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1619,41 +1674,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" thickBot="1">
+    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="e" cm="1">
+      <c r="B1" s="18" t="str" cm="1">
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C1" s="28" t="e">
+        <v>Converting</v>
+      </c>
+      <c r="C1" s="28" t="str">
         <f ca="1">"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
-        <v>#VALUE!</v>
+        <v>Save As Converting_test_cases.xlsx</v>
       </c>
       <c r="D1" s="29"/>
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
       <c r="G1" s="29"/>
     </row>
-    <row r="2" spans="1:7" ht="24">
+    <row r="2" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
@@ -1668,7 +1723,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="27" thickBot="1">
+    <row r="3" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -1691,7 +1746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="39.6">
+    <row r="4" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>11</v>
       </c>
@@ -1710,7 +1765,7 @@
       </c>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:7" ht="39.6">
+    <row r="5" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>11</v>
       </c>
@@ -1729,7 +1784,7 @@
       </c>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:7" ht="36">
+    <row r="6" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
         <v>11</v>
       </c>
@@ -1748,7 +1803,7 @@
       </c>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:7" ht="36">
+    <row r="7" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
@@ -1769,7 +1824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="65.45" customHeight="1">
+    <row r="8" spans="1:7" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
         <v>11</v>
       </c>
@@ -1788,7 +1843,7 @@
       </c>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>11</v>
       </c>
@@ -1809,7 +1864,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>11</v>
       </c>
@@ -1829,7 +1884,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="36">
+    <row r="11" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>11</v>
       </c>
@@ -1849,7 +1904,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="27" thickBot="1">
+    <row r="12" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>11</v>
       </c>
@@ -1868,7 +1923,7 @@
       </c>
       <c r="G12"/>
     </row>
-    <row r="13" spans="1:7" ht="27" thickBot="1">
+    <row r="13" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="26" t="s">
         <v>31</v>
       </c>
@@ -1880,10 +1935,10 @@
         <v>2</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="27" thickBot="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
@@ -1906,121 +1961,302 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15">
-      <c r="A15" s="16"/>
-      <c r="B15" s="17"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" ht="15">
-      <c r="A16" s="16"/>
-      <c r="B16" s="17"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" ht="15">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" ht="15">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" ht="15">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="13"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" thickBot="1">
-      <c r="A20" s="16"/>
-      <c r="B20" s="17"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="13"/>
-    </row>
-    <row r="21" spans="1:7" ht="27" thickBot="1">
-      <c r="A21" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="27" thickBot="1">
-      <c r="A22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="15">
-      <c r="A23" s="16"/>
-      <c r="B23" s="17"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="13"/>
-    </row>
-    <row r="24" spans="1:7" ht="15">
-      <c r="A24" s="16"/>
-      <c r="B24" s="17"/>
+    <row r="15" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="21">
+        <v>1</v>
+      </c>
+      <c r="D15" s="30">
+        <v>1</v>
+      </c>
+      <c r="E15" s="22"/>
+      <c r="F15" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="21">
+        <v>333</v>
+      </c>
+      <c r="D16" s="30">
+        <v>333</v>
+      </c>
+      <c r="E16" s="12"/>
+      <c r="F16" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="21">
+        <v>999999999</v>
+      </c>
+      <c r="D17" s="30">
+        <v>999999999</v>
+      </c>
+      <c r="E17" s="12"/>
+      <c r="F17" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="21">
+        <v>2789456235</v>
+      </c>
+      <c r="D18" s="30">
+        <v>2147483647</v>
+      </c>
+      <c r="E18" s="12"/>
+      <c r="F18" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="21">
+        <v>123.56</v>
+      </c>
+      <c r="D19" s="30">
+        <v>123.56</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="30">
+        <v>0</v>
+      </c>
+      <c r="E20" s="12"/>
+      <c r="F20" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="30">
+        <v>123</v>
+      </c>
+      <c r="F21" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="30">
+        <v>0</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="21">
+        <v>1.23648645555756E+17</v>
+      </c>
+      <c r="D23" s="24">
+        <v>1.23648645555756E+17</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="21">
+        <v>1.23456987123666E+17</v>
+      </c>
+      <c r="D24" s="24">
+        <v>1.23456987123666E+17</v>
+      </c>
       <c r="E24" s="2"/>
-      <c r="F24" s="13"/>
-    </row>
-    <row r="25" spans="1:7" ht="15">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17"/>
+      <c r="F24" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="2">
+        <v>123365479922112</v>
+      </c>
+      <c r="D25" s="24">
+        <v>123365479922112</v>
+      </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:7" ht="15">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="13"/>
-    </row>
-    <row r="27" spans="1:7" ht="15">
+      <c r="F25" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26"/>
+      <c r="F26" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="16"/>
       <c r="B27" s="17"/>
       <c r="E27" s="2"/>
       <c r="F27" s="13"/>
     </row>
-    <row r="28" spans="1:7" ht="15">
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="16"/>
       <c r="B28" s="17"/>
       <c r="E28" s="2"/>
       <c r="F28" s="13"/>
     </row>
+    <row r="61" spans="1:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B62" s="27"/>
+      <c r="C62" s="27"/>
+      <c r="D62" s="27"/>
+      <c r="E62" s="27"/>
+      <c r="F62" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A62:E62"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F1048576">
@@ -2185,13 +2421,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B3A1B7D-D95E-47A7-B30E-D2F430E11D75}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B3A1B7D-D95E-47A7-B30E-D2F430E11D75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02A89564-090C-4AB3-82D0-1F9A04E789E6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02A89564-090C-4AB3-82D0-1F9A04E789E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{928A5758-548A-49CA-8056-B2ACE5BFBA0F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{928A5758-548A-49CA-8056-B2ACE5BFBA0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a45da267-33a0-44df-a473-ed84a5818b2b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>